<commit_message>
Creating a query-recipe pair evaluation bank
</commit_message>
<xml_diff>
--- a/output/average_ratings_semantic.xlsx
+++ b/output/average_ratings_semantic.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="127">
   <si>
     <t>Query</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
     <t>body</t>
   </si>
   <si>
@@ -62,6 +65,168 @@
   </si>
   <si>
     <t>what can I make for a romantic dinner</t>
+  </si>
+  <si>
+    <t>coffee brandy cream brulee</t>
+  </si>
+  <si>
+    <t>creme brulee for two</t>
+  </si>
+  <si>
+    <t>easy creme brulee</t>
+  </si>
+  <si>
+    <t>lavender creme brulee</t>
+  </si>
+  <si>
+    <t>no fail creme brulee</t>
+  </si>
+  <si>
+    <t>authentic bolognese sauce  sugo alla bolognese</t>
+  </si>
+  <si>
+    <t>bolognese</t>
+  </si>
+  <si>
+    <t>spaghetti bolognese vegetarian</t>
+  </si>
+  <si>
+    <t>vegan bolognese</t>
+  </si>
+  <si>
+    <t>vegan creamy spaghetti bolognese</t>
+  </si>
+  <si>
+    <t>apple pie  1</t>
+  </si>
+  <si>
+    <t>apple pie dessert</t>
+  </si>
+  <si>
+    <t>apple pie with a crust</t>
+  </si>
+  <si>
+    <t>bread pudding apple pie</t>
+  </si>
+  <si>
+    <t>sheila s apple pie</t>
+  </si>
+  <si>
+    <t>best ever chocolate cake   recipe</t>
+  </si>
+  <si>
+    <t>chocolate  cake</t>
+  </si>
+  <si>
+    <t>delicious chocolate cake</t>
+  </si>
+  <si>
+    <t>most chocolatey chocolate cake</t>
+  </si>
+  <si>
+    <t>the best chocolate cake</t>
+  </si>
+  <si>
+    <t>fresh minted lemonade</t>
+  </si>
+  <si>
+    <t>fresh raspberry lemonade</t>
+  </si>
+  <si>
+    <t>most refreshing lemonade you will ever taste    quick   easy</t>
+  </si>
+  <si>
+    <t>old fashioned  fresh lemonade</t>
+  </si>
+  <si>
+    <t>healthy  quick  easy breakfast</t>
+  </si>
+  <si>
+    <t>quick   easy low cal breakfast or lunch</t>
+  </si>
+  <si>
+    <t>quick rice sandwich</t>
+  </si>
+  <si>
+    <t>the quick snack</t>
+  </si>
+  <si>
+    <t>two tin lunch</t>
+  </si>
+  <si>
+    <t>easy no yeast pizza dough</t>
+  </si>
+  <si>
+    <t>no yeast homemade pizza</t>
+  </si>
+  <si>
+    <t>pizza dough  with no yeast</t>
+  </si>
+  <si>
+    <t>pizza without the red sauce</t>
+  </si>
+  <si>
+    <t>rice pizza</t>
+  </si>
+  <si>
+    <t>absolutely guilt free lazy morning pancakes</t>
+  </si>
+  <si>
+    <t>chinese pancakes   no egg or milk</t>
+  </si>
+  <si>
+    <t>fat free pancake</t>
+  </si>
+  <si>
+    <t>milk free  egg free pancakes</t>
+  </si>
+  <si>
+    <t>pancakes   milk free</t>
+  </si>
+  <si>
+    <t>basic pasta dough  no egg</t>
+  </si>
+  <si>
+    <t>breakfast pasta</t>
+  </si>
+  <si>
+    <t>eggless pasta</t>
+  </si>
+  <si>
+    <t>fresh egg pasta gluten free</t>
+  </si>
+  <si>
+    <t>homemade  fat free  pasta</t>
+  </si>
+  <si>
+    <t>beef and rice stroganoff</t>
+  </si>
+  <si>
+    <t>beginner s rice</t>
+  </si>
+  <si>
+    <t>brazilian style beef strogonoff</t>
+  </si>
+  <si>
+    <t>sopa de pollo con arroz  chicken and rice soup</t>
+  </si>
+  <si>
+    <t>sopa seca de arroz  mexican rice</t>
+  </si>
+  <si>
+    <t>mirj s apres pta chicken dinner</t>
+  </si>
+  <si>
+    <t>romantic chicken scallopine with saffron cream sauce</t>
+  </si>
+  <si>
+    <t>romantic stuffed chicken breasts a deux</t>
+  </si>
+  <si>
+    <t>sensual chicken with champagne</t>
+  </si>
+  <si>
+    <t>valentines day recipe</t>
   </si>
   <si>
     <t xml:space="preserve">coffee brandy cream brulee
@@ -2534,13 +2699,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2556,940 +2721,1108 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="E5">
+        <v>0.5773502691896257</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>4.666666666666667</v>
-      </c>
-      <c r="D5">
-        <v>0.5773502691896257</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9">
         <v>4.333333333333333</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.154700538379252</v>
       </c>
-      <c r="E9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11">
         <v>4.333333333333333</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.154700538379252</v>
       </c>
-      <c r="E11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12">
         <v>3.333333333333333</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1.527525231651947</v>
       </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13">
         <v>4.333333333333333</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1.154700538379252</v>
       </c>
-      <c r="E13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15">
         <v>3.666666666666667</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0.5773502691896257</v>
       </c>
-      <c r="E15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16">
         <v>5</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17">
         <v>4.666666666666667</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.5773502691896257</v>
       </c>
-      <c r="E17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18">
         <v>4.666666666666667</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0.5773502691896257</v>
       </c>
-      <c r="E18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19">
         <v>5</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20">
         <v>5</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21">
         <v>5</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>0</v>
       </c>
-      <c r="E22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23">
         <v>5</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24">
         <v>3.666666666666667</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>1.154700538379251</v>
       </c>
-      <c r="E24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25">
         <v>4.333333333333333</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>1.154700538379252</v>
       </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>0</v>
       </c>
-      <c r="E26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27">
         <v>2.666666666666667</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>1.154700538379251</v>
       </c>
-      <c r="E27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28">
         <v>5</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>0</v>
       </c>
-      <c r="E28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>43</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29">
         <v>4.333333333333333</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>1.154700538379252</v>
       </c>
-      <c r="E29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
         <v>44</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30">
         <v>2.666666666666667</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>2.081665999466133</v>
       </c>
-      <c r="E30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
         <v>45</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31">
         <v>4</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>1.732050807568877</v>
       </c>
-      <c r="E31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
         <v>46</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36">
         <v>0.3333333333333333</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
         <v>51</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37">
         <v>1.333333333333333</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>1.527525231651947</v>
       </c>
-      <c r="E37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
         <v>52</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38">
         <v>2</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>1.732050807568877</v>
       </c>
-      <c r="E38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B39" t="s">
         <v>53</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
         <v>54</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40">
         <v>2</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>1.732050807568877</v>
       </c>
-      <c r="E40" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
         <v>55</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41">
         <v>2</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>1.732050807568877</v>
       </c>
-      <c r="E41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42">
         <v>5</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>0</v>
       </c>
-      <c r="E42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
         <v>57</v>
       </c>
-      <c r="C43">
-        <v>0</v>
+      <c r="C43" t="s">
+        <v>112</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
-      <c r="E43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
         <v>58</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44">
         <v>5</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>0</v>
       </c>
-      <c r="E44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
         <v>59</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45">
         <v>0.3333333333333333</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
         <v>60</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46">
         <v>4.666666666666667</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
         <v>61</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47">
         <v>5</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>0</v>
       </c>
-      <c r="E47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
         <v>62</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
         <v>63</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49">
         <v>4.666666666666667</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>0.5773502691896257</v>
       </c>
-      <c r="E49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
         <v>64</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50">
         <v>1.333333333333333</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>1.527525231651947</v>
       </c>
-      <c r="E50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
         <v>65</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>0.5773502691896258</v>
       </c>
-      <c r="E51" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
         <v>66</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D52">
         <v>4</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>1</v>
       </c>
-      <c r="E52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
         <v>67</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53">
         <v>5</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>0</v>
       </c>
-      <c r="E53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
         <v>68</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54">
         <v>5</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>0</v>
       </c>
-      <c r="E54" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
         <v>69</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55">
         <v>5</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>0</v>
       </c>
-      <c r="E55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
         <v>70</v>
       </c>
-      <c r="C56">
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56">
         <v>4.333333333333333</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>1.154700538379251</v>
       </c>
-      <c r="E56" t="s">
-        <v>71</v>
+      <c r="F56" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a easy way to add new reviews to the bank: via missing_reviews_bank
</commit_message>
<xml_diff>
--- a/output/average_ratings_semantic.xlsx
+++ b/output/average_ratings_semantic.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="181">
   <si>
     <t>Query</t>
   </si>
@@ -2278,6 +2278,428 @@
     <t xml:space="preserve">
         You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
         Here is the recipe: 
+        coffee brandy cream brulee
+Recipe posted on: 2005-11-19
+Tags: time-to-make, course, main-ingredient, preparation, occasion, desserts, eggs-dairy, 1-day-or-more, oven, refrigerator, dinner-party, holiday-event, eggs, broil, dietary, christmas, thanksgiving, low-sodium, low-in-something, equipment
+Description: a light custard with coffee and a light brandy flavor with a crunchy brown sugar topping. plan a day ahead the custard needs to chill overnight, the complete recipe can be doubled to make 12 you will need 6 ramekins or oven-proof custard cups (12 if you are doubling) to make this recipe, taken from bon appetit magazine
+This recipe takes 1440 minutes to be done.
+For this recipe you will need the ingredients: 
+whipping cream
+sugar
+instant coffee granules
+egg yolks
+brandy
+pure vanilla extract
+light brown sugar
+The 18 steps to make this recipe are: 
+set oven to 350 degrees f
+arrange 6 ramekins or use custard cups in a 13 x 9-inch baking dish
+in a medium saucepan combine cream and 1 / 4 cup sugar
+bring almost to a simmer 
+stirring until the sugar dissolves
+remove from heat and add in the coffee granules 
+whisk to dissolve the granules
+in a medium bowl whisk together egg yolks
+gradually whisk in the warm cream mixture 
+then the brandy and vanilla
+strain the custard into a 4-cup measuring cup then divide / pour the mixture evenly between the ramekins or custard cups
+pour enhough hot water into the 13x9 pan to come halfway up the sides of the ramekins
+bake the custards until center moves only slighty when the pan is shaken gently
+remove the ramekins from the pan
+cool slightly and then place in refrigerator for 3 hours
+remove from fridge 
+cover with plastic wrap 
+and continue to chill overnight
+the following day: preheat the broiler
+arrange the ramekins on a small sheet
+shake about 2-3 teaspoons brown sugar through a small strainer onto the top of each custard forming a layer
+broil about 6 inches from heat until the sugar melts 
+bubbles and carmalizes (watch closely and rotate the sheet for even browning
+refrigerate custards until sugar topping gets hard 
+at least 1 hour or up to 4 hours before serving
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        Brûlée Cream
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        creme brulee for two
+Recipe posted on: 2008-09-15
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, preparation, for-1-or-2, low-protein, 5-ingredients-or-less, desserts, eggs-dairy, easy, dietary, low-sodium, low-in-something, number-of-servings
+Description: yummy, easy creme brulee for two.  i wanted to find a good recipe for just the two of us, so i adapted recipes until i came up with this one.  you can easily multiply the ingredients for more (but leave the vanilla extract at a teaspoon).  sinfully delicious served with sliced fresh strawberries on top.  hubby asks for more as soon as he sees the ramekins in the dish rack drying!
+This recipe takes 45 minutes to be done.
+For this recipe you will need the ingredients: 
+heavy cream
+sugar
+egg yolks
+vanilla extract
+The 14 steps to make this recipe are: 
+preheat oven to 300 degrees
+heat heavy cream and 1 / 4 cup sugar over high heat until little bubbles form around the edges
+remove from heat
+whisk egg yolks and vanilla in a bowl 
+then add a tiny bit of cream mixture while whisking
+continue adding cream mixture bit by bit until gone
+"you dont want to add the hot cream mixture all at once because itll cook the yolks"
+pour into two creme brulee ramekins
+place ramekins in a baking dish with edges taller than the ramekins
+carefully pour enough water into the baking dish to halfway cover the sides of the ramekins
+be sure not to get water in the ramekins
+bake for 40 minutes
+carefully remove from oven and let cool
+remove ramekins from baking dish 
+cover with clear wrap 
+and refrigerate for at least 3-4 hours
+when ready to serve 
+sprinkle 1 / 2 tablespoon of sugar evenly over each ramekin 
+and torch in slow 
+steady circles until sugar caramelizes
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        Brûlée Cream
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        easy creme brulee
+Recipe posted on: 2005-11-29
+Tags: time-to-make, course, main-ingredient, preparation, low-protein, 5-ingredients-or-less, desserts, eggs-dairy, easy, beginner-cook, puddings-and-mousses, eggs, dietary, low-sodium, low-in-something, 4-hours-or-less
+Description: a very easy creme brulee with only 4 servings.
+This recipe takes 90 minutes to be done.
+For this recipe you will need the ingredients: 
+heavy cream
+egg yolks
+sugar
+vanilla extract
+light brown sugar
+The 13 steps to make this recipe are: 
+preheat oven to 275 degrees
+whisk the cream 
+egg yolks 
+sugar 
+and vanilla extract together in a bowl
+mix it all up until it gets nice and creamy
+pour this mixture into 4 ramekins
+place the ramekins in a baking pan
+fill the baking pan with hot water 
+about halfway up the sides of the ramekins
+place the pan with the ramekins in the oven for 45 minutes to an hour or so
+after 45 minutes or so check them every ten minutes
+"youll know theyre done when you can stick a knife in one and it comes out clean"
+remove the ramekins from the baking pan 
+set them on the counter 
+and let them cool for 15 minutes or so
+sprinkle a thin layer of the light brown sugar on the top of each
+"make sure its a thin layer 
+but also make sure it completely covers the custard"
+"now torch it ! or 
+if you dont have a torch 
+you can put them under the broiler for a minute or so"
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        Brûlée Cream
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        lavender creme brulee
+Recipe posted on: 2005-01-27
+Tags: time-to-make, course, preparation, 5-ingredients-or-less, desserts, easy
+Description: a deliciously fragrant custard, delicately enhanced with fresh lavender flowers. the perfect spring or summertime dessert, or anytime! use fresh organic lavender from your garden (or storebought culinary lavender).  cook time includes one hour stand time and several hours chill time. from pastry chef jack fisher at nine-ten restaurant in la jolla, ca.
+This recipe takes 320 minutes to be done.
+For this recipe you will need the ingredients: 
+heavy cream
+lavender flowers
+egg yolks
+sugar
+The 14 steps to make this recipe are: 
+preheat oven to 300 degrees
+in a saucepan 
+heat cream and lavender flowers over very low heat until warm
+remove from heat and let stand for one hour
+reheat before proceeding
+in a bowl 
+whisk egg yolks and 1 / 3 cup sugar 
+and add 1 cup warm cream
+add remaining cream and whisk until mixed thoroughly
+strain and pour into 4-inch ramekins
+place ramekins in a large roasting pan and pour enough hot water into pan to come halfway up sides of ramekins
+cover pan with foil and carefully transfer pan to oven
+bake custards for 45 to 50 minutes
+cool 
+then chill several hours
+when ready to serve 
+sprinkle about 2 teaspoons of sugar on top of each custard
+use a hand-held torch to melt the sugar or place the custards 6 inches below a broiler for 4 to 6 minutes 
+until sugar bubbles and turns golden brown
+refrigerate briefly 
+then serve
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        Brûlée Cream
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        no fail creme brulee
+Recipe posted on: 2010-02-16
+Tags: weeknight, time-to-make, course, main-ingredient, cuisine, preparation, occasion, for-1-or-2, desserts, eggs-dairy, french, oven, european, dinner-party, holiday-event, vegetarian, puddings-and-mousses, eggs, dietary, low-sodium, low-in-something, equipment, number-of-servings, presentation, served-cold, 4-hours-or-less
+Description: creme brulee has the reputation of being a very difficult dessert to make, but the most difficult part is planning and patience. plan to make this recipe a day before you need it, and make sure you have something to do while you hang around the house waiting for it to bake. as long as you have the right equipment and don't rush this recipe, you'll find that it's a no-fail creme brulee. make sure you have the right equipment before you start. i recommend using two personal souffle ramekins (mine are approximately 4-5 inches in diameter and about an inch to 1 1/2 inches deep) and one baking dish large enough to hold them both; it is essential that the creme brulee is baked in a water bath. i use glass or correlle to hold my ramekins.
+This recipe takes 105 minutes to be done.
+For this recipe you will need the ingredients: 
+cream
+sugar
+egg yolks
+vanilla
+brown sugar
+The 19 steps to make this recipe are: 
+preheat the oven to 300 degrees
+warm the cream in a small saucepan
+"dont bring to a boil 
+just heat the cream"
+meanwhile beat the eggs well in a medium-sized bowl
+add the sugar and beat into the eggs
+when cream is heated 
+add gradually to the eggs while beating
+add vanilla while beating
+prepare the water bath by placing both ramekins in the chosen baking dish
+fill the dish with warm water so it reaches two thirds up the sides of the ramekins
+fill the ramekins with the liquid custard
+bake for 30 minutes at 300 degrees
+reduce oven temperature to 275 degrees 
+and bake for another 30 to 60 minutes until custard is set
+custard is set if it only has a pudding-like jiggle when you gently jostle the ramekin
+if it has a liquid-like slosh 
+keep baking at 275
+chill the custard for at least two hours
+add the garnish by covering the tops of the chilled custards with sugar
+preheat the broiler
+put the ramekins under the broiler for about a minute or two 
+leaving the oven or broiler door open
+in the alternative 
+caramelize the sugar with a creme brulee torch
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        Brûlée Cream
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        authentic bolognese sauce  sugo alla bolognese
+Recipe posted on: 2012-02-12
+Tags: weeknight, time-to-make, course, main-ingredient, cuisine, preparation, occasion, sauces, main-dish, condiments-etc, beef, vegetables, european, dinner-party, italian, comfort-food, oamc-freezer-make-ahead, veal, savory-sauces, ground-beef, meat, tomatoes, taste-mood, number-of-servings, presentation, served-hot, 4-hours-or-less
+Description: a rich, meaty, and zesty "ragu".  bolognese sauce is the backbone of northern italian cooking, and once you try it you'll never toss your spaghetti with store-bought pasta sauce again. however, there are as many recipe versions of this delicious slow-cooked sauce as there are cooks in the italian city of bologna.  the secret ingredient  to a true bolognese sauce is milk (or cream), which is added in such small amount, you don't even know it's there. tip: bolognese sauce is best made the day before to allow the flavors to develop. cool the sauce, uncovered, and then refrigerate in an airtight container. can also be frozen.
+This recipe takes 120 minutes to be done.
+For this recipe you will need the ingredients: 
+onions
+carrots
+celery ribs
+garlic clove
+bacon
+extra virgin olive oil
+salt
+fresh ground pepper
+dried basil
+dried oregano
+dried thyme leaves
+ground veal
+dry white wine
+tomato paste
+crushed tomatoes
+milk
+ground nutmeg
+The 13 steps to make this recipe are: 
+place the chopped onions 
+carrots 
+celery 
+and garlic clove in a food processor
+pulse the motor until the vegetables are finely chopped
+heat the olive oil in a large 
+heavy saucepan set over medium heat
+add the chopped vegetables and chopped bacon
+stir in the salt 
+pepper 
+basil 
+oregano 
+and thyme
+cook 
+stirring occasionally 
+until vegetables are softened 
+about 5 minutes
+add the ground veal to the pot with the vegetables
+cook over medium-high heat 
+breaking up the meat with a wooden spoon 
+until the meat is no longer pink 
+about 6 minutes
+stir in the wine 
+tomato paste 
+crushed tomatoes 
+and the milk
+add the pinch of ground nutmeg
+reduce the heat to low and simmer gently 
+stirring occasionally 
+for 1 1 / 2 hours
+serve over spaghetti 
+cooked al dente 
+and pass the grated parmesan cheese
+mangia !
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        I'm vegan. How can I make a bolognese?
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        bolognese
+Recipe posted on: 2004-08-11
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, main-dish, vegetables, european, italian, dietary, meat, pasta-rice-and-grains, presentation, served-hot
+Description: i got this recipe from one of my mom's cookbooks.
+This recipe takes 15 minutes to be done.
+For this recipe you will need the ingredients: 
+olive oil
+bacon
+onion
+celery
+carrot
+garlic
+fresh thyme
+ground beef
+ground pork
+dry red wine
+bay leaves
+beef broth
+tomato puree
+pappardelle pasta
+parmesan cheese
+The 18 steps to make this recipe are: 
+heat oil in heavy large pot over medium high heat
+add bacon
+saut until beginning to brown 
+about 6 minutes
+add onion 
+celery 
+carrot 
+garlic 
+and thyme
+saut 5 minutes
+add beef and pork
+saut until brown and cooked through 
+breaking up meat with back of fork 
+about 10 minutes
+add wine and bay leaves
+simmer until liquid is slightly reduced 
+about 10 minutes
+add broth and tomato puree
+reduce heat to medium low
+simmer until sauce thickens 
+stirring often 
+about 1 hour 15 minutes
+season with salt and pepper
+boil pasta in large pot of boiling salted water until just tender but still firm to bite 
+stirring often
+drain
+transfer to pot with sauce
+toss
+serve with parmesan
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        I'm vegan. How can I make a bolognese?
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        spaghetti bolognese vegetarian
+Recipe posted on: 2002-05-29
+Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, main-dish, pasta, easy, vegetarian, dietary, pasta-rice-and-grains, spaghetti, novelty
+Description: i like this recipe because it taste like a meaty bolognese sauce,and it is a recipe made by myself 10 years ago.
+This recipe takes 30 minutes to be done.
+For this recipe you will need the ingredients: 
+textured vegetable protein
+water
+onions
+garlic
+carrots
+curry powder
+mixed spice
+parsley
+cumin powder
+oil
+tomato paste
+tomato sauce
+salt
+sugar
+spaghetti
+The 10 steps to make this recipe are: 
+fry onions in the oil until soft but not brown
+cut the carrots in small-diced 
+and add to the onions
+add the curry 
+spices and parsley
+add garlic
+stir in tomato paste 
+then tvp mixed with 3 cups water
+add salt and sugar
+fry 
+stirring occasionally until tvp is cooked
+add the tomatoes sauce
+serve on pasta with parmesan cheese
+it could be used for any pasta or lasghana
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        I'm vegan. How can I make a bolognese?
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
         vegan bolognese
 Recipe posted on: 2008-02-08
 Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, main-dish, pasta, dinner-party, vegetarian, dietary, comfort-food, pasta-rice-and-grains, spaghetti, taste-mood
@@ -2338,6 +2760,2001 @@
 User reviews: 
         Here is the query:
         I'm vegan. How can I make a bolognese?
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        vegan creamy spaghetti bolognese
+Recipe posted on: 2007-05-03
+Tags: lactose, 30-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, main-dish, pasta, vegetables, easy, european, beginner-cook, romantic, vegetarian, italian, stove-top, dietary, comfort-food, inexpensive, egg-free, free-of-something, pasta-rice-and-grains, spaghetti, tomatoes, taste-mood, equipment, presentation, served-hot
+Description: the only thing i can think to say about this is that it's really good!  eat it.
+This recipe takes 30 minutes to be done.
+For this recipe you will need the ingredients: 
+boca meatless ground burger
+diced tomatoes
+tomato sauce
+yellow onion
+vegan cream cheese
+dried thyme
+vegetable oil
+spaghetti
+The 8 steps to make this recipe are: 
+heat the oil in a pan over medium heat
+add the recipes crumbles and onion to the pan and saut until the crumbles are defrosted and the onions are softened
+add the diced tomatoes 
+tomato sauce and thyme
+"simmer the sauce for 15 minutes 
+taste and add more thyme if its needed"
+while the sauce is simmering 
+cook the spaghetti until al dente
+drain and return to the pot
+when the 15 minutes is up 
+add the vegan cream cheese and stir well to combine
+let it simmer for a few more minutes 
+then pour onto the pasta and toss
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        I'm vegan. How can I make a bolognese?
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        apple pie  1
+Recipe posted on: 2000-03-13
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, low-protein, pies-and-tarts, desserts, fruit, oven, pies, dietary, low-in-something, apples, equipment
+Description: to answer the reviewer who questioned the lack of apples, i believe this is what is called "mock apple pie."  that is, it tastes like apple pie but uses no apples.  my grandmother makes something like this.  that said, this is not my recipe.  it is an adopted recipe that i have asked be removed from my account, along with all other adoptees.  most were removed, but a couple were apparently missed.
+This recipe takes 35 minutes to be done.
+For this recipe you will need the ingredients: 
+unbaked pie crusts
+water
+sugar
+cream of tartar
+ritz crackers
+butter
+cinnamon
+nutmeg
+lemon
+juice and rind of
+The 14 steps to make this recipe are: 
+make your favorite pie crust
+boil water 
+sugar and cream of tartar
+add whole crackers 
+1 at a time
+boil 2 minutes
+add remaining ingredients
+cool
+pour into prepared pie shell
+cover with top crust
+slit top for steam vents
+bake at 425 degrees for 10 minutes
+reduce heat to 350 degrees
+continue to bake 20 to 25 minutes or until golden brown
+remove from oven
+cool
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        apple pie
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        apple pie dessert
+Recipe posted on: 2007-04-27
+Tags: time-to-make, course, main-ingredient, preparation, occasion, low-protein, very-low-carbs, pies-and-tarts, desserts, eggs-dairy, fruit, oven, easy, beginner-cook, dinner-party, holiday-event, kid-friendly, pies, dietary, christmas, low-sodium, low-cholesterol, low-saturated-fat, low-calorie, comfort-food, low-carb, inexpensive, low-in-something, apples, taste-mood, equipment, 4-hours-or-less
+Description: this is a simple yet delicious dessert that is wonderful served warm with ice cream, this can also be baked in a 9-inch square baking dish instead of the pie plate, throw in some raisins also ;-)
+This recipe takes 65 minutes to be done.
+For this recipe you will need the ingredients: 
+baking apples
+orange juice
+flour
+white sugar
+brown sugar
+cinnamon
+nutmeg
+salt
+butter
+vanilla ice cream
+The 9 steps to make this recipe are: 
+set oven to 375 degrees f
+lightly grease a 9-inch pie plate
+mound the apple slices in the pie plate 
+then sprinkle the orange juice over the apples
+in a medium bowl mix together flour 
+both sugars 
+cinnamon 
+nutmeg and salt
+add in cold butter cubes and mix together using your fingers until mixture resembles coarse crumbs
+scatter the mixture over the apples
+place the pie plate onto a baking sheet
+bake for about 40-45 minutes or until apples are tender but not too soft
+serve warm with vanilla ice cream if desired
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        apple pie
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        apple pie with a crust
+Recipe posted on: 2007-10-06
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, for-1-or-2, low-protein, healthy, 5-ingredients-or-less, beverages, fruit, easy, beginner-cook, dinner-party, holiday-event, low-fat, vegetarian, cocktails, dietary, new-years, low-sodium, low-cholesterol, low-saturated-fat, low-carb, healthy-2, low-in-something, apples, number-of-servings, 3-steps-or-less
+Description: this is really an adult cocktail. you can serve this warm or cold.
+This recipe takes 5 minutes to be done.
+For this recipe you will need the ingredients: 
+apple juice
+coconut rum
+cinnamon
+The 2 steps to make this recipe are: 
+mix all ingredients and serve either hot or cold
+sprinkle with cinnamon
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        apple pie
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        bread pudding apple pie
+Recipe posted on: 2003-09-10
+Tags: weeknight, time-to-make, course, main-ingredient, preparation, occasion, pies-and-tarts, desserts, fruit, oven, dinner-party, fall, holiday-event, vegetarian, pies, dietary, thanksgiving, seasonal, comfort-food, apples, taste-mood, sweet, equipment, 4-hours-or-less
+Description: want something different from the traditional apple pie? give this a try!
+This recipe takes 80 minutes to be done.
+For this recipe you will need the ingredients: 
+eggs
+applesauce
+non-fat vanilla yogurt
+white sugar
+brown sugar
+rolled oats
+ground cinnamon
+bread
+apples
+all-purpose flour
+butter
+9 inch pie shell
+The 8 steps to make this recipe are: 
+preheat oven to 350 degrees f
+in a medium mixing bowl stir together eggs 
+applesauce 
+yogurt 
+white sugar 
+1 / 2 cup brown sugar 
+oats 
+and cinnamon
+stir in bread and apples
+pour into pie crust
+in another bowl stir 1 / 4 cup brown sugar and flour
+cut in butter until mixture resembles coarse crumbs
+sprinkle on top of pie filling
+bake in preheated oven for 1 hour or until top is golden and fruit is tender
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        apple pie
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        sheila s apple pie
+Recipe posted on: 2009-08-24
+Tags: weeknight, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, low-protein, healthy, pies-and-tarts, desserts, fruit, american, easy, beginner-cook, fall, low-fat, pies, dietary, gifts, low-sodium, low-cholesterol, seasonal, low-saturated-fat, low-calorie, comfort-food, northeastern-united-states, low-in-something, apples, taste-mood, 4-hours-or-less
+Description: i could make this pie in my sleep, i have done it so many times!  it started out when my son was small and we used to go apple picking.  i had to use up all those apples so i made pies and gave them away.  suddenly, everyone else decided to go apple picking too and would bring me their apples to turn into pies!  it's just a basic, traditional recipe but it is delicious and homey.  note:  i will tell you that my preference is for cortland apples, and it ends up being about 2-1/2 lbs. usually.
+This recipe takes 70 minutes to be done.
+For this recipe you will need the ingredients: 
+apples
+lemon juice
+sugar
+flour
+salt
+cinnamon
+nutmeg
+butter
+pastry for double-crust pie
+The 13 steps to make this recipe are: 
+quarter 
+core and peel apples
+slice apples into a large bowl making sure not to cut them too thin
+toss apples with lemon juice
+in a small bowl 
+stir together sugar 
+flour 
+salt 
+cinnamon 
+and nutmeg
+pour over fruit and toss well to coat evenly
+roll out pastry for lower crust
+fit loosely into a 9-inch or 10-inch pie plate
+pile fruit into lower crust and dot with bits of butter
+roll out pastry for upper crust and fold in half
+slash a few times across fold to create vents for escape of steam
+lay pastry over fruit and trim 1 / 2 inch beyond edge of plate
+tuck upper crust under lower crust all around the edge and flute with fingers to seal 
+or seal by pressing down with tines of a fork all around the edge
+bake in a very well preheated 450 degree fahrenheit oven for 30 to 40 minutes or until fruit is tender and crust is nicely browned
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        apple pie
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        best ever chocolate cake   recipe
+Recipe posted on: 2008-06-08
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, south-west-pacific, desserts, australian, dinner-party, holiday-event, cakes, chocolate
+Description: i have won taste and presentation competitions with this cake and have been using this recipe for years.  this cake is the best ever!
+This recipe takes 55 minutes to be done.
+For this recipe you will need the ingredients: 
+unsalted butter
+caster sugar
+icing sugar
+eggs
+vanilla essence
+seedless blackberry jam
+self raising flour
+cocoa powder
+bicarbonate of soda
+milk
+The 9 steps to make this recipe are: 
+prepare round 20cm baking tin by buttering / oiling surface and the placing grease paper in base and sides
+using electric beaters 
+beat butter and sugar and sifted icing sugar in small mixing bowl until light and fluffy
+add eggs gradually beating thoroughly after each addition
+add essence and jam 
+beat until combined
+transfer mixture to large mixing bowl
+using a metal spoon 
+fold in sifted flour 
+cocoa and soda alternately with milk
+stir until just combined and the mixture is almost smooth
+pour into prepared tin 
+smooth surface
+bake for 45 minutes in 180 degrees celsius oven or until skewer comes out clean when inserted in centre
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        chocolate cake recipe
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        chocolate  cake
+Recipe posted on: 2007-02-26
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, desserts, canadian, easy, beginner-cook, potluck, kid-friendly, picnic, cakes, chocolate, dietary, comfort-food, toddler-friendly, taste-mood, sweet, to-go
+Description: this is our family's favorite chocolate cake.  
+the addition of coffee makes a rich tasting cake. also the oil instead of butter is healthier. i sometimes add grated orange peel.
+This recipe takes 35 minutes to be done.
+For this recipe you will need the ingredients: 
+flour
+sugar
+baking soda
+salt
+cocoa
+sour cream
+brewed coffee
+egg
+canola oil
+The 4 steps to make this recipe are: 
+mix dry ingredients
+add wet ingredients and beat well
+pour into greased 9 x 13 pan
+bake 350 for 30-35 minutes
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        chocolate cake recipe
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        delicious chocolate cake
+Recipe posted on: 2006-01-24
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, healthy, desserts, eggs-dairy, oven, easy, beginner-cook, dinner-party, holiday-event, kid-friendly, cakes, chocolate, dietary, inexpensive, brunch, taste-mood, sweet, equipment
+Description: truly a wonderful chocolate cake!  i make two of these and frost the middle and the outsides with frosting!
+This recipe takes 45 minutes to be done.
+For this recipe you will need the ingredients: 
+sugar
+butter
+egg
+cocoa powder
+vanilla
+flour
+baking powder
+baking soda
+boiling water
+The 9 steps to make this recipe are: 
+set oven to 350
+grease a 9 x 9-inch baking pan
+in a bowl cream the butter and sugar until light
+add in the egg and the cocoa / water mixture with vanilla
+mix until combined
+in a small bowl mix together the baking soda and 1 / 2 cup boiling water 
+then add in with the flour and baking powder
+mix until combined and smooth
+transfer to prepared baking dish
+bake for about 30 minutes or until the cake tests done
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        chocolate cake recipe
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        most chocolatey chocolate cake
+Recipe posted on: 2012-10-23
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, desserts, french, european, cakes, chocolate, birthday
+Description: this cake is the most moist and chocolatey chocolate cake i ever had!  i found this in a cookbook made by the hersheys company and it might taste better if you use their type of cocoa or icing.  it is incredibly delicious!
+This recipe takes 55 minutes to be done.
+For this recipe you will need the ingredients: 
+granulated sugar
+flour
+cocoa
+baking powder
+baking soda
+salt
+eggs
+milk
+vegetable oil
+vanilla extract
+boiling water
+butter
+powdered sugar
+The 19 steps to make this recipe are: 
+1
+preheat oven to 350 degrees celcius and grease and flour 2 nine inch pans
+2
+mix together sugar 
+flour 
+cocoa 
+baking powder 
+baking soda 
+and salt in large bowl
+3
+add eggs 
+milk 
+oil and vanilla
+beat on medium speed of mixer for 2 minutes
+4
+stir in boiling water 
+then pour batter into prepared pans
+5
+bake for 30-35 minutes or until wooden pick inserted in the middle comes out clean
+6
+cool for 10 minutes 
+then take out of pan and cool completely
+7
+ffor the icing - melt the butter 
+then stir in the cocoa
+add sugar and milk
+8
+spread icing on top of the bottom layer
+then put the top layer on and ice the top and sides
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        chocolate cake recipe
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        the best chocolate cake
+Recipe posted on: 2004-11-03
+Tags: 60-minutes-or-less, time-to-make, course, preparation, desserts, cakes, dietary
+Description: totally the best!
+This recipe takes 50 minutes to be done.
+For this recipe you will need the ingredients: 
+flour
+sugar
+unsweetened cocoa
+baking soda
+baking powder
+eggs
+milk
+vegetable oil
+vanilla
+boiling water
+The 6 steps to make this recipe are: 
+preheat ovento 350f prepare 2 round 9 inch cake pans by spraying with pam 
+then sprinkle with flour and tap out the extra
+in a large bowl sift all dry ingredients together
+in a smaller bowl combine eggs 
+milk 
+vanilla 
+water and oil
+mix with an electric hand mixer until combined
+add wet ingredients to the flour mixture and stir until well combined
+pour batter into pans and bake for 30-35 minutes
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        chocolate cake recipe
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        fresh lemonade
+Recipe posted on: 2003-07-23
+Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, low-protein, healthy, 5-ingredients-or-less, beverages, fruit, easy, refrigerator, holiday-event, low-fat, picnic, spring, summer, vegan, vegetarian, dietary, low-sodium, low-cholesterol, seasonal, low-saturated-fat, low-calorie, independence-day, healthy-2, low-in-something, citrus, lemon, to-go, equipment, number-of-servings
+Description: i like my lemonade more tart than sweet. adjust the amount of water and sugar to your taste.
+This recipe takes 25 minutes to be done.
+For this recipe you will need the ingredients: 
+sugar
+boiling water
+lemon juice
+water
+lemon slice
+The 5 steps to make this recipe are: 
+add sugar and boiling water to a pitcher
+stir until sugar dissolves
+add lemon juice and cold water
+stir to mix
+chill for several hours and serve over ice
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        fresh lemonade
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        fresh minted lemonade
+Recipe posted on: 2006-08-09
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, 5-ingredients-or-less, beverages, fruit, american, southwestern-united-states, easy, european, dinner-party, holiday-event, kid-friendly, dietary, citrus, lemon, brunch
+Description: ooh, with lots of mint! screams summer! adapted from cooks illustrated, their most popular recipes!
+This recipe takes 15 minutes to be done.
+For this recipe you will need the ingredients: 
+lemons
+fresh mint leaves
+granulated sugar
+salt
+cold water
+The 9 steps to make this recipe are: 
+mash lemons 
+mint leaves 
+and sugar in a large 
+deep bowl with potato masher or back of wooden spoon until lemon slices give up their juice 
+sugar is dissolved 
+and juice is thickened to syrup consistency 
+about 4 minutes
+pour half the lemon slices and syrup through a large sieve over bowl
+press on solids with masher or back of wooden spoon to release as much liquid as possible
+discard solids
+move liquid to serving pitcher
+repeat process with remaining lemon slices
+stir in water until blended
+chill well and stir to blend before serving 
+over ice
+enjoy !
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        fresh lemonade
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        fresh raspberry lemonade
+Recipe posted on: 2011-07-24
+Tags: weeknight, 30-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, low-protein, healthy, beverages, fruit, american, southern-united-states, easy, holiday-event, kid-friendly, low-fat, vegan, vegetarian, dietary, low-sodium, low-cholesterol, low-saturated-fat, low-calorie, healthy-2, low-in-something, berries, raspberries, citrus, lemon, non-alcoholic
+Description: this is a make ahead kid friendly drink from cooking light august 2011. enjoy!
+This recipe takes 20 minutes to be done.
+For this recipe you will need the ingredients: 
+sugar
+water
+fresh raspberries
+fresh orange juice
+fresh lemon juice
+sparkling water
+The 11 steps to make this recipe are: 
+combine sugar and 3 / 4 cup water in a small saucepan
+bring to a boil
+cook 2 minutes 
+stirring until sugar dissolves
+cool to room temperature
+combine remaining 1 1 / 4 cups water and raspberries in a blender
+pulse 10 times or until well blended
+strain mixture through a fine sieve into a large pitcher
+discard solids
+add orange juice 
+lemon juice 
+sparkling water 
+and cooled syrup to pitcher
+stir to combine
+serve immediately over ice
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        fresh lemonade
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        most refreshing lemonade you will ever taste    quick   easy
+Recipe posted on: 2002-08-02
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, low-protein, healthy, 5-ingredients-or-less, beverages, fruit, easy, no-cook, refrigerator, low-fat, picnic, summer, dietary, low-sodium, gluten-free, low-cholesterol, seasonal, low-saturated-fat, low-calorie, low-carb, free-of-something, low-in-something, to-go, equipment, number-of-servings, technique
+Description: this is the best tasting, most satisfying, easiest homemade lemonade you will ever drink. what could be more satisfying on a hot summer day than the cool, brisk refreshing taste of lemonade? this is so easy with the help of a citrus juicer to juice the lemons.
+This recipe takes 5 minutes to be done.
+For this recipe you will need the ingredients: 
+fresh lemon juice
+sugar
+club soda
+lemon
+The 4 steps to make this recipe are: 
+combine lemon juice 
+sugar and club soda stirring well to dissolve sugar
+add sliced lemon to pitcher
+chill
+enjoy !
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        fresh lemonade
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        old fashioned  fresh lemonade
+Recipe posted on: 2006-03-08
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, low-protein, healthy, beverages, fruit, american, southern-united-states, easy, beginner-cook, holiday-event, low-fat, summer, dietary, low-sodium, low-cholesterol, seasonal, low-saturated-fat, low-calorie, independence-day, healthy-2, low-in-something, citrus, lemon, lime, 3-steps-or-less
+Description: summers in sw florida can get quite oppressive, and few things are as rejuvenating as this thirst-quenching drink on a steamy afternoon. sit back, put your feet up, and pour over ice.
+This recipe takes 10 minutes to be done.
+For this recipe you will need the ingredients: 
+sugar
+boiling water
+fresh lemon juice
+cold water
+lemon slice
+mint sprig
+The 4 steps to make this recipe are: 
+stir together sugar and 1 / 2 cup boiling water until sugar dissolves
+stir in lemon juice and 5 cups cold water
+garnish 
+if desired
+fresh limeade: substitute fresh lime juice for lemon juice
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        fresh lemonade
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        healthy  quick  easy breakfast
+Recipe posted on: 2008-11-27
+Tags: 15-minutes-or-less, time-to-make, course, preparation, occasion, for-1-or-2, 5-ingredients-or-less, breakfast, lunch, snacks, easy, vegetarian, dietary, brown-bag, to-go, number-of-servings, 3-steps-or-less
+Description: i try to work out in the mornings, and this is a light breakfast that won't bog me down but gives me the energy to get through the work out.
+This recipe takes 4 minutes to be done.
+For this recipe you will need the ingredients: 
+fat free greek yogurt
+apple
+cinnamon
+agave nectar
+The 3 steps to make this recipe are: 
+chop the apple
+combine all ingredients in a bowl
+eat !
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        healthy recipe for quick lunch
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        quick   easy low cal breakfast or lunch
+Recipe posted on: 2001-10-13
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, north-american, for-1-or-2, healthy, 5-ingredients-or-less, breakfast, eggs-dairy, vegetables, canadian, oven, easy, low-fat, cheese, broil, dietary, low-sodium, gluten-free, low-cholesterol, low-saturated-fat, low-calorie, healthy-2, free-of-something, low-in-something, equipment, number-of-servings
+Description: i find this a very satisfying yet low cal breakfast. i would not eat these rice cakes until i tried them with something on them. experiment and find your own favorite.
+This recipe takes 9 minutes to be done.
+For this recipe you will need the ingredients: 
+rice cakes
+tomatoes
+hot sauce
+parmesan cheese
+salt and pepper
+The 4 steps to make this recipe are: 
+place tomato slices on the rice cakes
+sprinkle with hot sauce 
+salt and pepper
+drizzle with parmesan
+broil for about 3-4 minutes
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        healthy recipe for quick lunch
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        quick rice sandwich
+Recipe posted on: 2002-05-25
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, preparation, for-1-or-2, 5-ingredients-or-less, lunch, main-dish, eggs-dairy, rice, easy, microwave, cheese, dietary, sandwiches, pasta-rice-and-grains, equipment, number-of-servings
+Description: so you want a quick warm lunch sandwhich, but what is this? there's no bread in the bread box? no pitas? no tortillas? you need a quick fix, a sandwhichy solution, warm, and using cheese and meat. here it is!
+This recipe takes 2 minutes to be done.
+For this recipe you will need the ingredients: 
+cooked rice
+water
+meat
+fat free cheese
+The 6 steps to make this recipe are: 
+put rice and water in microwaveable container 
+cover with paper towel 
+and cook until steaming
+drain water and add cheese and meat
+do not cover
+place back into microwave for about 30 more seconds
+cheese should be somewhat melty
+mix with fork and eat
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        healthy recipe for quick lunch
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        the quick snack
+Recipe posted on: 2007-03-25
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, for-1-or-2, 5-ingredients-or-less, granola-and-porridge, breakfast, lunch, snacks, eggs-dairy, fruit, easy, no-cook, beginner-cook, dietary, berries, pasta-rice-and-grains, brunch, number-of-servings, 3-steps-or-less, technique
+Description: this is a fast, tasty, and it includes alot of your daily nutrients.
+This recipe takes 5 minutes to be done.
+For this recipe you will need the ingredients: 
+yogurt
+banana
+grapes
+berries
+cereal
+The 4 steps to make this recipe are: 
+take out a bowl and mix all the ingredients
+let stand for about 3 minutes 
+so the cereal absorbs a bit of the yogurt
+dont have to do that 
+but i like to
+then relax and enjoy !
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        healthy recipe for quick lunch
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        two tin lunch
+Recipe posted on: 2008-03-28
+Tags: 15-minutes-or-less, time-to-make, course, preparation, healthy, appetizers, lunch, easy, dietary, low-sodium, low-cholesterol, healthy-2, low-in-something, 3-steps-or-less
+Description: some thing else for lunch
+This recipe takes 10 minutes to be done.
+For this recipe you will need the ingredients: 
+tuna
+corn
+mayonnaise
+salt and pepper
+crispbread
+parsley sprig
+The 4 steps to make this recipe are: 
+mix the tuna 
+corn and mayonnaise together
+season to taste
+serve on crispbreads
+garnish with parsley if desired
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        healthy recipe for quick lunch
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        easy no yeast pizza dough
+Recipe posted on: 2007-09-19
+Tags: 60-minutes-or-less, time-to-make, course, preparation, 5-ingredients-or-less, flat-shapes, breads, main-dish, easy, vegan, vegetarian, pizza, dietary
+Description: i've made this several times and it always turns out good. make sure you knead the dough for the required 5-7 minutes. i have added dried herbs and onion flakes right into the dough as well.
+This recipe takes 50 minutes to be done.
+For this recipe you will need the ingredients: 
+spelt flour
+baking powder
+sea salt
+water
+olive oil
+The 21 steps to make this recipe are: 
+"preheat your oven to 400f"
+place the flour 
+baking powder and the salt into a bowl
+make a well in the center and add the water and oil
+combine by gradually incorporating the flour into the olive oil and water
+you may want to add a little more water if necessary
+transfer the dough to a floured board and knead it at least for 5-7 minutes
+let the dough rest in an air tight plastic bag while you prepare the toppings for your pizza
+once the toppings are made 
+set them aside and take the dough out of the plastic bag
+put a tiny bit of oil in the center of your pizza pan and with your hands and finger
+i use a 12 inch pizza pan
+you could probably stretch it to 15 inches 
+but it would be a thinner crust
+place your pizza sauce on the dough and then cover with your favorite toppings
+pop it into the preheated oven
+check it after about 20 minutes to see how the crust is browning
+some ovens are hotter then others 
+so this is a good habit to get into
+bon appetit !
+p
+s
+": if you change the ingredients in this recipe i cant guarantee its going to turn out the way mine did"
+but 
+hey 
+experiment with it
+thanks for choosing my recipe !
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        how to make a pizza without an oven
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        no yeast homemade pizza
+Recipe posted on: 2009-04-05
+Tags: 60-minutes-or-less, time-to-make, course, preparation, 5-ingredients-or-less, main-dish, easy, beginner-cook, vegetarian, pizza, dietary, inexpensive
+Description: easy pizza crust to make when you don't have yeast.
+This recipe takes 35 minutes to be done.
+For this recipe you will need the ingredients: 
+flour
+milk
+oil
+baking powder
+salt
+The 6 steps to make this recipe are: 
+preheat the oven 425 degrees f
+combine all ingredients and knead ten times
+let stand for ten minutes
+put dough on a cookie sheet and roll or press out
+top with toppings
+bake 20-25 minutes or until edges are golden
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        how to make a pizza without an oven
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        pizza dough  with no yeast
+Recipe posted on: 2004-02-25
+Tags: 30-minutes-or-less, time-to-make, course, preparation, breads, lunch, main-dish, oven, easy, pizza, dietary, inexpensive, equipment, number-of-servings
+Description: i like this recipe because it's simple and uses ingredients i always have on hand. i got it from my dad, i can't say for sure where it originally came from, but maybe from a betty crocker cookbook. this dough also works well for making meat pies.
+This recipe takes 30 minutes to be done.
+For this recipe you will need the ingredients: 
+flour
+baking powder
+salt
+milk
+salad oil
+The 10 steps to make this recipe are: 
+heat oven to 425f
+measure ingredients into a bowl
+stir vigorously until mixture leaves the side of the bowl
+gather dough together and press into a ball
+knead dough in bowl 10 times to make smooth then divide dough in half
+on lightly floured surface roll each half into a 13-inch circle
+place on pizza pan
+turn up edges 1 / 2 inch and pinch
+brush circles with remaining 2t of salad oil
+add toppings and bake for 20-25 minutes or until it looks done
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        how to make a pizza without an oven
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        pizza without the red sauce
+Recipe posted on: 2007-02-18
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, main-dish, vegetables, oven, european, vegetarian, pizza, dietary, taste-mood, to-go, equipment
+Description: still has a light tomato taste from the sun-dried tomato pesto.  recipe courtesy of aimee from allrecipes.com.
+This recipe takes 35 minutes to be done.
+For this recipe you will need the ingredients: 
+butter
+olive oil
+garlic
+sun-dried tomato pesto
+dried basil leaves
+dried oregano
+parmesan cheese
+pizza crust
+tomatoes
+fresh spinach
+sweet onion
+fresh jalapeno pepper
+feta cheese
+The 6 steps to make this recipe are: 
+preheat oven according to pizza crust package directions
+in a small bowl combine butter 
+olive oil 
+garlic 
+pesto 
+basil 
+oregano and parmesan cheese
+spread mixture evenly on pizza crust
+arrange tomato 
+spinach 
+onion and jalapeno on pizza
+top with crumbled feta cheese
+bake according to pizza crust package directions
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        how to make a pizza without an oven
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        rice pizza
+Recipe posted on: 2003-05-06
+Tags: 60-minutes-or-less, time-to-make, course, preparation, main-dish, pizza, dietary
+Description: a very low fat, and different approach to pizza. after not having pizza for a year and a half, this was a true blessing to my taste buds. you can top with your favorite pizza toppings. this is a recipe created by joanna lund. prep time does not include time needed to prepare the rice.
+This recipe takes 55 minutes to be done.
+For this recipe you will need the ingredients: 
+cooked rice
+eggs
+lowfat mozzarella cheese
+lean ground turkey
+onion
+fresh mushrooms
+tomato sauce
+italian seasoning
+fat-free parmesan cheese
+The 16 steps to make this recipe are: 
+preheat oven to 450 degrees
+spray a 12" pizza pan with cooking spray
+in a medium bowl 
+combine rice 
+eggs and 1 / 4 c mozzarella cheese
+mix well
+spread rice mixture evenly on pizza
+bake 20 minutes
+in a skillet 
+brown meat and onion
+remove from heat
+in a small bowl 
+combine tomato sauce and italian seasoning
+spread sauce evenly over baked crust
+top with meat mixture
+evenly sprinkle parmesan cheese and remaining mozzarella cheese over top
+bake an additional 10-15 minutes
+let set 5 minutes
+cut into 6 pieces
+2cups uncooked rice usually cooks to about 3 cups
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        how to make a pizza without an oven
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        absolutely guilt free lazy morning pancakes
+Recipe posted on: 2007-09-11
+Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, for-1-or-2, healthy, pancakes-and-waffles, breakfast, european, grains, dietary, pasta-rice-and-grains, number-of-servings
+Description: this is for pancake lovers who worry about their waists. very low-calorie and packed with goodness. must be enjoyed hot.
+This recipe takes 20 minutes to be done.
+For this recipe you will need the ingredients: 
+egg
+olive oil
+flax seeds
+sugar
+baking powder
+baking soda
+salt
+skim milk
+plain yogurt
+water
+vanilla extract
+quick oatmeal
+whole wheat flour
+The 16 steps to make this recipe are: 
+beat the egg with milk 
+sugar 
+youghurt 
+olive oil and water
+combine all dry ingredients in a bowl
+mix well
+add the dry mixture into the liquid and beat until smooth
+let stand for about 15 minute the batter must have a consistency of thin porridge
+add a table spoon of water if too thick
+brush a small non-stick pan with the greasing oil or spray with cooking spray
+spoon pancakes with a small ladle and cook on medium-high
+turn over when surface gets bubbly
+no need to respray if your pan is truly non-stick
+this makes 6 pancakes that are fluffy 
+tender and yummy
+117 cal / pancake
+serve with fruits 
+low-cal youghurt or eggs
+i love dipping them into a soft-boiled egg
+optional: if you intend to serve them with fruits like apples or bananas 
+add a pinch of cinnamon and nutmeg into the batter
+the heat will enhance the spices
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pancake without flour and milk
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        chinese pancakes   no egg or milk
+Recipe posted on: 2008-04-09
+Tags: lactose, 60-minutes-or-less, time-to-make, course, cuisine, preparation, occasion, healthy, 5-ingredients-or-less, appetizers, side-dishes, asian, easy, dinner-party, low-fat, dietary, low-sodium, low-cholesterol, low-saturated-fat, egg-free, healthy-2, free-of-something, low-in-something, brunch
+Description: these lovely light pancakes are great with duck, and contain no egg or dairy
+This recipe takes 35 minutes to be done.
+For this recipe you will need the ingredients: 
+plain flour
+water
+sesame oil
+salt
+The 8 steps to make this recipe are: 
+sift the flour and salt into a mixing bowl 
+add the water and mix until they form a dough
+knead lightly on a floured surface and divide into 12 equal pieces
+roll out into circles the size of tea plates
+lightly brush the surface of 6 circles with the oil on one side
+cover each one carefully with another circle and roll out gently
+fry the pancakes in a dry frying pan or griddle over a medium heat for 3 -4 minutes 
+turning once 
+until firm but not too brown
+cool for a few minutes then peel the pancakes apart
+they can be made in advance and stored in an airtight container until needed
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pancake without flour and milk
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        fat free pancake
+Recipe posted on: 2006-06-20
+Tags: 15-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, for-1-or-2, healthy, 5-ingredients-or-less, pancakes-and-waffles, breakfast, easy, diabetic, low-fat, dietary, low-cholesterol, low-saturated-fat, comfort-food, egg-free, free-of-something, low-in-something, taste-mood, number-of-servings
+Description: a healthy yummy breakfast treat for those avoiding fat. this makes one large pancake. you can multiply the recipe for multiple servings.
+This recipe takes 7 minutes to be done.
+For this recipe you will need the ingredients: 
+whole wheat flour
+baking soda
+salt
+vanilla extract
+milk
+The 5 steps to make this recipe are: 
+mix first four ingredients and enough milk to make a runny batter
+spray a pan with olive oil spray
+pour batter onto pan
+fry on each side at medium heat for about 45 seconds
+top with berries 
+honey 
+etc
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pancake without flour and milk
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        milk free  egg free pancakes
+Recipe posted on: 2004-06-04
+Tags: lactose, 30-minutes-or-less, time-to-make, course, preparation, pancakes-and-waffles, breakfast, easy, beginner-cook, kid-friendly, dietary, inexpensive, free-of-something
+Description: my oldest daughter was severely allergic to milk for three+ years, then *poof* the allergy ceased to exist in her system. while she had this allergy, we struggled with milk-free recipes/food. i began making nearly everything from scratch. i bought a really great book, the milk-free kitchen, where this recipe is from. we still make these soft, fluffy and delicious pancakes. i will also post the recipe for milk-free blueberry pancakes.
+This recipe takes 20 minutes to be done.
+For this recipe you will need the ingredients: 
+white flour
+white sugar
+baking powder
+salt
+margarine
+water
+eggs
+The 14 steps to make this recipe are: 
+sift flour 
+sugar 
+baking powder 
+and salt together into medium mixing bowl
+melt 2 1 / 2 tbsp margarine in frying pan until melted
+be sure to
+pour melted margarine in a small bowl 
+add water and egg
+mix well
+stir liquid mixture into the dry ingredients until it is thoroughly moistened
+it is ok if this batter is lumpy
+cook the pancakes over medium-high heat on the stove-top
+cook pancakes until the tops are bubbly and the bottoms browned
+turn the pancakes over to cook other side
+serve hot with margarine 
+honey 
+brown sugar or maple syrup
+actual cooking time will depend on the size of the pan you are using
+i have a small frying pan 
+so i have to do these individually
+my mom has a griddle large enough to cook them all at once
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pancake without flour and milk
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        pancakes   milk free
+Recipe posted on: 2007-06-09
+Tags: 30-minutes-or-less, time-to-make, course, preparation, pancakes-and-waffles, breakfast, dietary, low-saturated-fat, free-of-something, low-in-something
+Description: these pancakes are from the dairy free cookbook, by jane zukin.   my 1 year old grandson is allergic to milk and it is very hard to find recipes for him.  he loves these pancakes!
+This recipe takes 25 minutes to be done.
+For this recipe you will need the ingredients: 
+flour
+baking powder
+sugar
+salt
+egg
+orange juice
+water
+vegetable oil
+vegetable oil cooking spray
+The 7 steps to make this recipe are: 
+mix together flour 
+baking powder 
+sugar and salt
+combine egg 
+orange juice 
+water and oil
+add liquid to dry ingredients 
+stirring just until moist
+let mixture rest for 30 seconds
+spoon or pour batter onto greased 
+hot griddle
+cook pancakes on the first side until bubbles appear on upper surface
+turn over and cook until bottom is golden
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pancake without flour and milk
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        basic pasta dough  no egg
+Recipe posted on: 2009-03-11
+Tags: time-to-make, main-ingredient, preparation, healthy, 5-ingredients-or-less, pasta, easy, dietary, low-sodium, low-cholesterol, low-saturated-fat, egg-free, healthy-2, free-of-something, low-in-something, pasta-rice-and-grains, 4-hours-or-less
+Description: this recipe yields the equivalent of about 1-1/2 lbs of dry pasta, and can be used to make 4 dozen raviolis.
+This recipe takes 120 minutes to be done.
+For this recipe you will need the ingredients: 
+flour
+warm water
+olive oil
+The 7 steps to make this recipe are: 
+put flour in large mixing bowl 
+making a well in the center
+add wet ingredients to well and very slowly mix together with a fork 
+incorporating only a little flour at a time so it mixes smoothly and evenly
+trust me 
+the more patient you are with this the better it will turn out
+continue kneading by hand for about 10 minutes 
+let rest for a half hour covered with a towel
+repeat a couple times until dough is smooth and silky 
+and just slightly sticky
+shape by hand or with a machine
+depending on the shape 
+cook for 30 seconds to 2 minutes
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pasta without eggs
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        breakfast pasta
+Recipe posted on: 2002-06-12
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, breakfast, lunch, main-dish, eggs-dairy, pasta, vegetables, easy, kid-friendly, cheese, eggs, stove-top, dietary, low-sodium, comfort-food, inexpensive, low-in-something, pasta-rice-and-grains, taste-mood, equipment
+Description: we have always eaten pasta for breakfast - leftover or fresh cooked - with tomato sauce or chicken broth and cheese. this is the ultimate recipe. imagine serving this at your next brunch (lunch or dinner). from the little tree b&amp;b, taos, nm.
+This recipe takes 35 minutes to be done.
+For this recipe you will need the ingredients: 
+spaghettini
+olive oil
+butter
+garlic
+fresh mushrooms
+green onions
+roma tomatoes
+eggs
+fresh parsley
+fresh basil
+parmesan cheese
+The 9 steps to make this recipe are: 
+while pasta is cooking 
+saute garlic and mushrooms in 1 tablespoon olive oil
+before mushrooms are thoroughly cooked 
+add green onions 
+remove from heat and reserve for later use
+crack eggs into bowl and lightly beat
+when pasta is cooked 
+drain
+in large skillet melt butter with 1 tablespoon olive oil 
+add pasta to skillet and stir briefly
+add eggs and half of the parmesan cheese 
+stir until eggs begin to form curds on pasta
+then add garlic 
+mushrooms 
+green onions 
+basil 
+and chopped parsley
+lastly 
+add chopped tomatoes 
+stirring briefly to incorporate
+immediately place on serving plates and sprinkle with fresh ground black pepper and rest of cheese
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pasta without eggs
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        eggless pasta
+Recipe posted on: 2003-01-13
+Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, healthy, 5-ingredients-or-less, pasta, easy, beginner-cook, kid-friendly, low-fat, vegan, vegetarian, stove-top, dietary, low-cholesterol, low-saturated-fat, comfort-food, healthy-2, low-in-something, pasta-rice-and-grains, taste-mood, equipment, number-of-servings
+Description: this recipe is posted by request. original poster is webby.
+This recipe takes 17 minutes to be done.
+For this recipe you will need the ingredients: 
+semolina flour
+salt
+water
+The 7 steps to make this recipe are: 
+in a large bowl mix together flour and salt
+slowly stir in the warm water and mix until a stiff dough is formed
+lightly flour your counter top or board and turn out dough
+knead for 10 minutes 
+adding a touch of water if the dough is too stiff to work with
+form into a ball 
+cover and let rest for 20 minutes
+at this point you can roll it out and cut into desired shapes or run through a pasta machine
+boil a large pot of salted water 
+drop in pasta and cook for 4 minutes 
+drain and serve
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pasta without eggs
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        fresh egg pasta gluten free
+Recipe posted on: 2003-04-23
+Tags: 30-minutes-or-less, time-to-make, main-ingredient, preparation, occasion, pasta, holiday-event, kosher, vegetarian, lasagna, stove-top, dietary, gluten-free, passover, free-of-something, pasta-rice-and-grains, spaghetti, equipment
+Description: this recipe from 
+This recipe takes 30 minutes to be done.
+For this recipe you will need the ingredients: 
+tapioca flour
+cornstarch
+potato starch
+salt
+xanthan gum
+eggs
+vegetable oil
+The 15 steps to make this recipe are: 
+in a medium bowl 
+combine flours 
+salt 
+and xanthan gum
+beat the eggs lightly and add the oil
+pour the egg-oil liquid into the flour mixture and stir
+this will feel much like pastry dough
+work the dough into a firm ball
+knead for 1 or two minutes
+place the ball of dough on a potato starch-floured breadboard and roll asthin as possible
+this dough is tough and 
+when almost transparent 
+will still handle well
+cut into desired shape
+for fettuccine and spaghetti 
+slice very thin strips
+for a noodle casserole 
+make slightly wider noodles
+if using for lasagne 
+cut into 1 1 / 2-by-4-inch rectangles
+to cook pasta: cook in salted boiling water 
+to which 1 tablespoon of oil has been added 
+for about 10 to 12 minutes depending on the thickness and size of your pieces
+you will have to test for doneness
+drain and rinse well
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pasta without eggs
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        homemade  fat free  pasta
+Recipe posted on: 2001-12-14
+Tags: weeknight, time-to-make, preparation, healthy, 5-ingredients-or-less, easy, low-fat, dietary, low-sodium, low-cholesterol, low-saturated-fat, healthy-2, low-in-something, 4-hours-or-less
+Description: you need a pasta machine(manual or electric)directions are for a manual one
+This recipe takes 90 minutes to be done.
+For this recipe you will need the ingredients: 
+all-purpose flour
+fat free egg substitute
+The 13 steps to make this recipe are: 
+put the flour into the bowl of a food processor
+pulse while adding the egg substitute
+this will produce a soft ball of dough
+turn out onto a floured towel or board and knead the dough into a single ball that is glossy and elastic
+put in plastic wrap and set aside for 30 minutes
+flour the rollers of a pasta machine
+cut the dough in quarters
+flour all over and flatten
+put the first piece of dough through the largest opening on the pasta machine 3 times 
+folding the dough in half after each time through
+then put it through each successively smaller opening until it has gone through the smallest
+repeat this process for the remaining 3 pieces of dough
+put each of the thin pieces of dough through the wide cutters on machine
+hang and dry 10 minutes
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        pasta without eggs
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        beef and rice stroganoff
+Recipe posted on: 2004-03-20
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, preparation, main-dish, beef, rice, dietary, one-dish-meal, low-carb, ground-beef, low-in-something, meat, pasta-rice-and-grains
+Description: my favorite rice-a-roni stroganoff mix was discontinued and i was looking for a replacement for the recipe on the box using ground beef. so, i found a basic ground beef stroganoff recipe and adapted it. my husband says it's even better than the boxed one, and i agree. hope you do too.
+This recipe takes 45 minutes to be done.
+For this recipe you will need the ingredients: 
+fresh mushrooms
+onion
+lean ground beef
+salt
+garlic
+dry sherry
+beef broth
+minute rice
+sour cream
+fresh ground pepper
+The 6 steps to make this recipe are: 
+in large skillet on medium heat 
+start browning ground beef 
+breaking it up as it cooks
+when partially cooked 
+add salt 
+onions 
+garlic 
+and mushrooms and continue cooking until soft and ground beef browns
+add sherry to deglaze
+add beef broth and minute rice 
+bring to boil 
+cover and simmer 10 minutes
+check rice and if needed 
+simmer another 5 minutes
+stir in sour cream and heat through 
+add pepper to taste
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        strogonoff with rice
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        beginner s rice
+Recipe posted on: 2007-03-20
+Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, low-protein, healthy, 5-ingredients-or-less, side-dishes, rice, asian, easy, beginner-cook, low-fat, romantic, dietary, low-cholesterol, low-saturated-fat, low-calorie, comfort-food, inexpensive, low-in-something, pasta-rice-and-grains, white-rice, taste-mood
+Description: for some reason, folks are afraid to try to make white rice unless it comes pre-packaged in a packet or a box (not bulk). here's a fool-proof recipe that will have you making rice as a side dish three nights a week. i've been making it this way for years and i mostly use basmati rice that i buy in the big bags. however, i also frequently use the cheap, plain white rice that comes in 2 and 3-pound plastic bags and this recipe works just fine.
+This recipe takes 25 minutes to be done.
+For this recipe you will need the ingredients: 
+white rice
+tap water
+butter
+salt
+The 8 steps to make this recipe are: 
+in a 3-quart saucepan 
+bring the water 
+salt 
+and butter to a rolling boil
+add in the dry rice and stir
+reduce the heat to very low 
+a simmer 
+and cover
+check the rice after 12 minutes and stir
+"if its gooey-looking or still wet 
+re-cover and check it again in 5 more minutes"
+it should be done at this point
+fluff it up with a spoon and take it off the heat
+"cover again until youre ready to serve"
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        strogonoff with rice
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        brazilian style beef strogonoff
+Recipe posted on: 2008-04-03
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, main-dish, beef, brazilian, stove-top, south-american, dietary, one-dish-meal, stir-fry, comfort-food, oamc-freezer-make-ahead, low-carb, low-in-something, meat, steak, taste-mood, savory, equipment, number-of-servings, presentation, served-hot, technique
+Description: this is a brazilian favorite and one of our family's too! beef strogonoff comes in a flavor-rich heavy cream sauce, with a touch of ketchup, mustard and soy sauce, along with chopped mushrooms. it is perfect when served with white rice, potato sticks and a green salad.
+i particularly am not very fond of mushrooms, so i leave it out of the recipe when i make it for my picky eaters at home, but i am posting the original recipe for this brazilian dish. enjoy!
+This recipe takes 50 minutes to be done.
+For this recipe you will need the ingredients: 
+butter
+filet mignon
+onion
+mushroom
+soy sauce
+cognac
+table cream
+ketchup
+mustard
+flour
+milk
+The 20 steps to make this recipe are: 
+season filet mignon with salt and pepper to taste
+in a medium pan 
+saut seasoned filet mignon in high heat with butter
+reserve
+in a bigger pan 
+brown onion with butter and then add the mushrooms and the reserved steak
+let it cook for about 5 minutes
+add the soy sauce and the cognac 
+and singe it
+in a bowl 
+mix the table cream 
+ketchup 
+mustard 
+salt and pepper to taste and the flour dissolved in milk 
+and add this mixture to the steak and mushrooms and let it cook for 5-8 more minutes in medium heat until the sauce incorporates and thickens
+turn off heat and serve the strogonoff with potato sticks 
+white rice and a nice salad
+beef: let the steak rest about 1-2 hours 
+out of the fridge before preparing the dish
+"the beef has to saut and not cook 
+so it is best to brown it in high heat and dont let it release too much juice in the pan 
+preserving its color 
+moisture and flavor"
+heating up the cognac: get a coffee cup half full of hot water and set a snifter across the top
+it will heat it perfectly
+heating it in a microwave 
+open flame or steam should all produce the same end result
+table cream: to take the watery part of the canned table cream 
+let the can sit in the fridge for about 4 hours prior to using it 
+and when you open the can 
+it will be easier to separate the cream from the runny part
+in doing that 
+the strogonoff will be creamier and thicker
+if you use the fresh heavy cream 
+let the sauce cook for a little more to thicken
+to freeze: this recipe can be made and frozen but do not add the table cream when freezing
+after taking the prepared steak out of the freezer 
+add the table cream and heat it up prior to serving
+)
+you may substitute steak for chicken breast 
+shrimp 
+cod fish 
+and sliced tuna
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        strogonoff with rice
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        sopa de pollo con arroz  chicken and rice soup
+Recipe posted on: 2001-01-29
+Tags: weeknight, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, soups-stews, poultry, mexican, heirloom-historical, holiday-event, chicken, dietary, meat, 4-hours-or-less
+Description: this mexican soup recipe cheerfully stolen from: mario's la fiesta mexican restaurant in berkeley, ca.
+This recipe takes 240 minutes to be done.
+For this recipe you will need the ingredients: 
+whole chicken
+russet potato
+carrots
+tomatoes
+celery
+garlic cloves
+salt
+white onion
+rice
+cannonball cabbage
+cilantro
+ground cumin
+white pepper
+crystal hot sauce
+water
+The 34 steps to make this recipe are: 
+extract giblets from chicken and remove the liver
+place chicken in a pot of water just large enough to hold it
+cover with 1-2 quarts of water and add the giblets
+add salt and bring to a boil 
+skimming off any foam
+reduce heat 
+cover pot 
+and simmer for 20 or more minutes
+chicken should fall apart after cooking
+completely bone out the cooked chicken
+separate white meat for use in the finished soup
+crack the bones and return them to the stock with the skin
+add all other non-meat parts of the chicken back to the stock
+bring stock and giblets back to a fast simmer
+cook stock for 1 / 2-1 hour longer
+begin washing rice
+strain stock and remove most 
+but not all of the fat
+peel the potato 
+tomato and carrots
+bring stock to a boil and reduce heat
+cut carrots into coins 
+dice potato into 1 / 2" cubes and add with cabbage cut into 1" chunks
+chop onion coarsely and add along with pressed or finely minced garlic
+remove strings by breaking the top of the stalk backwards and pulling down to strip them out 
+slice celery into medium pieces and add
+peel and seed tomato 
+strain tomato juice from seeds and add with chopped cilantro leaves
+chop some of the celery heart\s leaves and add with diced chicken white meat in 1 / 2" chunks
+finish washing rice and add to soup
+during last half hour of cooking add all other spices
+adjust salt to taste
+avoid adding too much cumin 
+it will spoil the flavor
+do not let the soup boil 
+it will turn to mush
+do not use the chicken liver in the soup
+when the rice begins to "bloom" turn off the heat
+elbow macaroni 
+stars or alphabet pasta may be used
+if using pasta 
+omit or reduce the amount of rice
+if the stock is made right it will gel when chilled
+do not use chicken bullion cubes or paste when making this
+they will cloud the soup and destroy its delicate bouquet
+tinned broth is acceptable but will not compare to using the stock described above
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        strogonoff with rice
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        sopa seca de arroz  mexican rice
+Recipe posted on: 2007-02-19
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, north-american, side-dishes, rice, mexican, inexpensive, pasta-rice-and-grains, white-rice, long-grain-rice
+Description: my bf said this was the best rice he had ever eaten. i adapted this recipe from a sunset mexican cookbook. this recipe can easily be cut in half.
+This recipe takes 60 minutes to be done.
+For this recipe you will need the ingredients: 
+long grain rice
+butter
+onions
+garlic cloves
+tomatoes
+regular-strength chicken broth
+chilies
+fresh cilantro
+pimento stuffed olive
+The 8 steps to make this recipe are: 
+in a wide frying pan over medium-high heat 
+brown rice lightly in butter or margarine
+add onion 
+garlic 
+tomato 
+and chiles 
+if used and cook for 2 or 3 minutes
+add 3 cups of the broth
+cover and simmer 25 to 35 minutes or bake 
+covered 
+in a 350f oven 50 to 60 minutes
+add more broth 
+if needed 
+to cook rice
+however 
+there should be no liquid remaining when rice is tender to bite
+add cilantro 
+if desired 
+during last 10 minutes
+garnish rice with olives
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        strogonoff with rice
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        mirj s apres pta chicken dinner
+Recipe posted on: 2002-06-17
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, main-dish, poultry, vegetables, potluck, dinner-party, holiday-event, kosher, romantic, chicken, dietary, low-sodium, gluten-free, low-cholesterol, low-saturated-fat, low-calorie, stir-fry, low-carb, healthy-2, free-of-something, low-in-something, meat, taste-mood, to-go, technique
+Description: this recipe is part of the june 2002 ready set cook contest. i was trapped in a boring pta meeting and started writing out ideas for recipes. a friend of mine was looking over my shoulder and said, "thanks, this is what we are going to have for dinner after this meeting!" voila!
+This recipe takes 45 minutes to be done.
+For this recipe you will need the ingredients: 
+boneless skinless chicken breasts
+button mushroom
+balsamic vinegar
+artichoke hearts
+fresh broccoli
+garlic cloves
+onion
+olive oil
+sweet paprika
+brown sugar
+salt and pepper
+ground ginger
+water
+The 18 steps to make this recipe are: 
+season the chicken breasts with salt and pepper
+you can pound them flat or leave them thick 
+as you prefer
+heat 2 tablespoons of olive oil in a teflon skillet 
+and sear the breasts 
+4 minutes on each side 
+until cooked through
+if you leave the chicken breasts thick this may take a little longer
+remove the cooked breasts from the pan and keep warm
+chop the broccoli into small florets
+coarsely chop the onions and mince the garlic
+cut the mushrooms into quarters
+if they are small you can cut them into halves
+coarsely chop the artichoke hearts
+heat the remaining 2 tablespoons of oil
+add the onions and saute until slightly softened and golden
+add the rest of the chopped vegetables and the garlic
+stir fry together for about 8 minutes
+add the balsamic vinegar 
+paprika 
+ginger 
+brown sugar 
+more salt and pepper to taste 
+and the water
+bring to a boil 
+lower the heat and cook and reduce the liquid 
+about 10 minutes altogether
+place each chicken breast on a plate and top with the vegetables
+serve with plain rice and a green salad
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        what can I make for a romantic dinner
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        romantic chicken scallopine with saffron cream sauce
+Recipe posted on: 2009-02-16
+Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, very-low-carbs, main-dish, poultry, european, holiday-event, romantic, italian, chicken, dietary, seasonal, low-calorie, low-carb, valentines-day, low-in-something, meat, taste-mood
+Description: this is a recipe of giada de laurentiis's from foodnetwork.com (but i lessened the salt, added flour, upped the garlic, and added a sauce-thickening tip). it seems like it would be super hard, but it is really not that difficult. the first time i made it was for my husband on valentine's day. i had never cooked with several of the ingredients before, and except accidentally buying chicken tenders instead of chicken cutlets, it turned out just lovely. :) i also found saffron threads the cheapest at whole foods, almost $7.00 less expensive than the next cheapest place! i served this over angel hair pasta with green beans and garlic breadsticks, and we had recipe #175610 for dessert.
+This recipe takes 30 minutes to be done.
+For this recipe you will need the ingredients: 
+olive oil
+chicken cutlet
+shallots
+garlic cloves
+white wine
+chicken broth
+saffron thread
+heavy cream
+salt
+fresh ground black pepper
+flour
+flat-leaf italian parsley
+The 14 steps to make this recipe are: 
+warm the olive oil in a large skillet over high heat
+season the chicken cutlets with salt and pepper 
+and coat each side with flour
+cook the chicken until golden and cooked through 
+about 2 to 3 minutes per side
+transfer the chicken to serving plate and tent with foil to keep warm
+turn the heat to medium 
+add the shallots and the garlic and cook until tender 
+about 2 minutes
+deglaze the pan with the white wine
+using a wooden spoon 
+scrape all the brown bits from the bottom of the pan
+cook until the wine is almost evaporated
+add the chicken broth and saffron threads 
+bring to a simmer and reduce for 10 minutes
+add the cream 
+salt 
+and pepper
+stir to combine and simmer for 1 minute to blend the flavors
+if you want an even thicker sauce 
+you can mix 1 tablespoon cornstarch with 1 tablespoon water 
+and add it to the pan
+pour the sauce over the chicken
+sprinkle with parsley and serve immediately
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        what can I make for a romantic dinner
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        romantic stuffed chicken breasts a deux
+Recipe posted on: 2006-07-04
+Tags: 60-minutes-or-less, time-to-make, course, main-ingredient, preparation, occasion, for-1-or-2, main-dish, poultry, dinner-party, holiday-event, kosher, romantic, chicken, dietary, wedding, passover, valentines-day, meat, chicken-breasts, taste-mood, number-of-servings
+Description: first, a little information:  sushiman and i have 8 kids together.  a meal alone at home with just the two of us is usually a non-existant event.  but last night the planets were aligned correctly, and it was just the two of us.  we had originally planned to go out for a quick bite to eat, but i decided to take advantage of the privacy and cook us a romantic dinner.  i had no idea what to make, but the inspiration just came to me while i was in the supermarket.  this recipe is an original creation that evolved as i was making it last night.  i'm so impressed with myself i just had to share it with you.  the quantities here are just enough for two, but you can double (triple, quadruple) the ingredients for the amount of people you want to feed.
+This recipe takes 35 minutes to be done.
+For this recipe you will need the ingredients: 
+chicken breasts
+roasted red peppers
+pastrami
+salt
+fresh ground black pepper
+sweet paprika
+oil
+The 9 steps to make this recipe are: 
+preheat your oven to 375 degrees f
+pour a bit of oil in a small baking dish
+lay out the two flattened chicken breasts
+cut the roasted pepper lengthwise down the side so you can lay it flat on top of the chicken breast
+place two slices of smoked meat on top of each roasted pepper
+roll up the chicken breast 
+lay seam side down in the oiled baking dish
+sprinkle with salt 
+pepper and paprika
+bake uncovered for about 20-25 minutes
+serve with a vegetable and a green salad on the side
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        what can I make for a romantic dinner
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        sensual chicken with champagne
+Recipe posted on: 2006-01-26
+Tags: 30-minutes-or-less, time-to-make, course, main-ingredient, cuisine, preparation, occasion, north-american, main-dish, poultry, vegetables, american, dinner-party, holiday-event, romantic, chicken, stove-top, one-dish-meal, stir-fry, valentines-day, mushrooms, meat, carrots, taste-mood, equipment, presentation, served-hot, technique
+Description: i came up with this recipe because i made sharon 123's recipe for recipe #144056 and thought it would enhance this dish nicely. of course you can use olive oil.  i was going for a chicken paprikash dish without the fat of sour cream and add lots of veggies like carrots, mushrooms and onions. makes it a light dish for valentines day--saves room to share a sensual dessert for two!
+This recipe takes 30 minutes to be done.
+For this recipe you will need the ingredients: 
+flour
+seasoning salt
+sweet paprika
+chicken breast
+olive oil
+baby carrots
+mushrooms
+sweet onion
+garlic cloves
+champagne
+tomato paste
+fresh parsley
+fresh thyme
+parsley
+thyme
+The 11 steps to make this recipe are: 
+mix the first 3 ingredient together
+coat tenderized chicken with the flour mixture and let sit to absorb while stir frying veggies
+in a very large non stick pan 
+heat oil and stir fry carrots 
+mushrooms 
+and onions 2 minutes over high heat add garlic stirring constantly for 3 more minute
+remove veggies and keep warm
+in the same pan brown one side of chicken adding oil only if needed for 1 minute
+flip and top with the cooked veggies cooking for 2 minutes
+pour in the champagne cook for 3 minutes
+add herbs and stir in paste cook till the champagne is reduced in half and sauce is glistening
+season with salt and pepper if needed
+garnish with fresh herbs
+serve over white rice or noodles
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        what can I make for a romantic dinner
+        Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
+        Assistant grading:
+        Justificative:
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        You are a query result validator assistant tasked with evaluating the quality of a given recipe in answering a given query.
+        Here is the recipe: 
+        valentines day recipe
+Recipe posted on: 2015-01-11
+Tags: time-to-make, preparation, occasion, for-1-or-2, easy, holiday-event, valentines-day, number-of-servings, 4-hours-or-less
+Description: on valentine’s day, indulge your night with a sexy, easy and delicious three course meal for you and your special someone.
+This recipe takes 80 minutes to be done.
+For this recipe you will need the ingredients: 
+apple
+strawberries
+fresh pineapple chunk
+orange
+white corn syrup
+fresh mint leaves
+sugar
+heavy cream
+bittersweet chocolate
+butter
+cabernet sauvignon wine
+fresh strawberries
+fresh cherries
+soy sauce
+mirin
+salmon fillets
+jasmine rice
+vegetable oil
+The 22 steps to make this recipe are: 
+for the fruit cups:
+in a bowl 
+combine apples 
+strawberries 
+pineapple 
+orange and corn syrup and mix well
+cover and refrigerate for 4 hours
+just before serving 
+garnish with fresh mint leaves
+for the chocolate fondue:
+in a microwave-safe bowl 
+mix the sugar 
+heavy cream 
+chocolate 
+and butter together and microwave for 2 minute
+take out of microwave and give it a quick whisk
+add wine and whisk again
+transfer to a fondue pot with a flame underneath
+serve with strawberries and cherries on the side 
+for dipping
+for the salmon teriyaki and jasmine rice:
+in a shallow container 
+mix the soy sauce 
+mirin and sugar until the sugar dissolves
+coat both sides of the salmon with the mixture and arrange pieces skin side up in the container
+refrigerate for 30 min to 1 hour
+in the meantime 
+cook the rice according to package directions
+arrange your oven racks so that the skillet you will be cooking in is as close as possible to the broiler flame
+turn on the broiler
+preheat a cast iron or other ovenproof skillet over high heat on the stove until very hot
+remove the salmon from the marinade and brush both sides with the oil
+place the salmon skin side up in the skillet and transfer the pan to the broiler
+cook for 1 to 2 min and check for doneness
+"if it isnt done 
+flip and cook for 1 min more"
+The mean rating for this recipe is: No reviews
+User reviews: 
+        Here is the query:
+        what can I make for a romantic dinner
         Now evaluate from 0 to 5, the relevance of the recipe for answering the given query, where 0 is unrelated, 1 is poorly related, 2 is a little relevant but miss some important things, 3 is relevant but miss some restrictions, 4 is a relevant recipe that nearly matches all the possible criterias, and 5 is a perfect result, where every possible consideration and restrain included in the query is answered in the recipe. Include both your grading and a brief justificative of the grade.
         Assistant grading:
         Justificative:
@@ -2762,7 +5179,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2782,7 +5199,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2802,7 +5219,7 @@
         <v>0.5773502691896257</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2822,7 +5239,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2842,7 +5259,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2862,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2882,7 +5299,7 @@
         <v>1.154700538379252</v>
       </c>
       <c r="F9" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2902,7 +5319,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2922,7 +5339,7 @@
         <v>1.154700538379252</v>
       </c>
       <c r="F11" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2942,7 +5359,7 @@
         <v>1.527525231651947</v>
       </c>
       <c r="F12" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2962,7 +5379,7 @@
         <v>1.154700538379252</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2982,7 +5399,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F14" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3002,7 +5419,7 @@
         <v>0.5773502691896257</v>
       </c>
       <c r="F15" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3022,7 +5439,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3042,7 +5459,7 @@
         <v>0.5773502691896257</v>
       </c>
       <c r="F17" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3062,7 +5479,7 @@
         <v>0.5773502691896257</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3082,7 +5499,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3102,7 +5519,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3122,7 +5539,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3142,7 +5559,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3162,7 +5579,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3182,7 +5599,7 @@
         <v>1.154700538379251</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3202,7 +5619,7 @@
         <v>1.154700538379252</v>
       </c>
       <c r="F25" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3222,7 +5639,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3242,7 +5659,7 @@
         <v>1.154700538379251</v>
       </c>
       <c r="F27" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3262,7 +5679,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3282,7 +5699,7 @@
         <v>1.154700538379252</v>
       </c>
       <c r="F29" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3302,7 +5719,7 @@
         <v>2.081665999466133</v>
       </c>
       <c r="F30" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3322,7 +5739,7 @@
         <v>1.732050807568877</v>
       </c>
       <c r="F31" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3342,7 +5759,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F32" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3362,7 +5779,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3382,7 +5799,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F34" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3402,7 +5819,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3422,7 +5839,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F36" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3442,7 +5859,7 @@
         <v>1.527525231651947</v>
       </c>
       <c r="F37" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3462,7 +5879,7 @@
         <v>1.732050807568877</v>
       </c>
       <c r="F38" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3482,7 +5899,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F39" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3502,7 +5919,7 @@
         <v>1.732050807568877</v>
       </c>
       <c r="F40" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3522,7 +5939,7 @@
         <v>1.732050807568877</v>
       </c>
       <c r="F41" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3542,7 +5959,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3562,7 +5979,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3582,7 +5999,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>126</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3602,7 +6019,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F45" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3622,7 +6039,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F46" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3642,7 +6059,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3662,7 +6079,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F48" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3682,7 +6099,7 @@
         <v>0.5773502691896257</v>
       </c>
       <c r="F49" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3702,7 +6119,7 @@
         <v>1.527525231651947</v>
       </c>
       <c r="F50" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3722,7 +6139,7 @@
         <v>0.5773502691896258</v>
       </c>
       <c r="F51" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3742,7 +6159,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -3762,7 +6179,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3782,7 +6199,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>126</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3802,7 +6219,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>126</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3822,7 +6239,7 @@
         <v>1.154700538379251</v>
       </c>
       <c r="F56" t="s">
-        <v>126</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>